<commit_message>
More cleanup/structuring of MAIN
- added profiler
- separated postprocessing, solver and scenario settings from MAIN
- choose between manual instance or excel input
</commit_message>
<xml_diff>
--- a/Data/emission_cap.xlsx
+++ b/Data/emission_cap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\home.ansatt.ntnu.no\egbertrv\Documents\GitHub\AIM_Norwegian_Freight_Model\Data\Reorganized\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/steffejb_ntnu_no/Documents/Work/GitHub/AIM_Norwegian_Freight_Model/AIM_Norwegian_Freight_Model/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E49E95E7-A7D8-49F5-9616-FF58770DCDB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{E49E95E7-A7D8-49F5-9616-FF58770DCDB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D72BC0B-BF01-4309-933B-2A94A8862112}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6291FB66-00B5-4A39-923B-42FCF76189FF}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="28800" windowHeight="23400" xr2:uid="{6291FB66-00B5-4A39-923B-42FCF76189FF}"/>
   </bookViews>
   <sheets>
     <sheet name="emission_cap" sheetId="1" r:id="rId1"/>
@@ -452,10 +452,13 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="5" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Objective function cost definition change
- Updated the objective function
- Demand is OK
- simplify the model
- CONTINUE DEBUGGING THE ExtractModelResults part
</commit_message>
<xml_diff>
--- a/Data/emission_cap.xlsx
+++ b/Data/emission_cap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/steffejb_ntnu_no/Documents/Work/GitHub/AIM_Norwegian_Freight_Model/AIM_Norwegian_Freight_Model/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{E49E95E7-A7D8-49F5-9616-FF58770DCDB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{936F106E-2B52-4203-B5F9-6C090818494F}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{E49E95E7-A7D8-49F5-9616-FF58770DCDB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A2AD059-BDF9-47CA-B761-85DFD4B6B955}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{6291FB66-00B5-4A39-923B-42FCF76189FF}"/>
+    <workbookView xWindow="14550" yWindow="0" windowWidth="43050" windowHeight="23400" xr2:uid="{6291FB66-00B5-4A39-923B-42FCF76189FF}"/>
   </bookViews>
   <sheets>
     <sheet name="emission_cap" sheetId="1" r:id="rId1"/>
@@ -517,7 +517,7 @@
         <v>2050</v>
       </c>
       <c r="B6">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed years: 2020, 2025 to 2022, 2026
Both in input files and in code
</commit_message>
<xml_diff>
--- a/Data/emission_cap.xlsx
+++ b/Data/emission_cap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/steffejb_ntnu_no/Documents/Work/GitHub/AIM_Norwegian_Freight_Model/AIM_Norwegian_Freight_Model/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\home.ansatt.ntnu.no\egbertrv\Documents\GitHub\AIM_Norwegian_Freight_Model\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{E49E95E7-A7D8-49F5-9616-FF58770DCDB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66D3E0CE-68E3-4183-8876-6D95B0ADF7A3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4AABF0D-65A5-43CB-B2B3-8E136BB701D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14550" yWindow="0" windowWidth="43050" windowHeight="23400" xr2:uid="{6291FB66-00B5-4A39-923B-42FCF76189FF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6291FB66-00B5-4A39-923B-42FCF76189FF}"/>
   </bookViews>
   <sheets>
     <sheet name="emission_cap" sheetId="1" r:id="rId1"/>
@@ -464,7 +464,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,7 +482,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -490,7 +490,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="B3">
         <v>75</v>
@@ -534,7 +534,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,7 +567,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -595,7 +595,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="B3">
         <v>75</v>

</xml_diff>

<commit_message>
Update penalties and emission targets
</commit_message>
<xml_diff>
--- a/Data/emission_cap.xlsx
+++ b/Data/emission_cap.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\home.ansatt.ntnu.no\egbertrv\Documents\GitHub\AIM_Norwegian_Freight_Model\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/steffejb_ntnu_no/Documents/Work/GitHub/AIM_Norwegian_Freight_Model/AIM_Norwegian_Freight_Model/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBCB3FC-22D3-4D19-AE40-ED17EFF9D4E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{8EBCB3FC-22D3-4D19-AE40-ED17EFF9D4E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E523E8D4-6CE8-48FA-86C6-C1BB9CC3C0D6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6291FB66-00B5-4A39-923B-42FCF76189FF}"/>
+    <workbookView xWindow="13800" yWindow="0" windowWidth="30345" windowHeight="23400" xr2:uid="{6291FB66-00B5-4A39-923B-42FCF76189FF}"/>
   </bookViews>
   <sheets>
     <sheet name="emission_cap" sheetId="1" r:id="rId1"/>
@@ -63,8 +63,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -92,8 +100,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,12 +473,12 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -484,7 +493,7 @@
       <c r="A2">
         <v>2022</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>100</v>
       </c>
     </row>
@@ -493,15 +502,16 @@
         <v>2026</v>
       </c>
       <c r="B3">
-        <v>80</v>
+        <f>B2/2+B4/2</f>
+        <v>72.5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2030</v>
       </c>
-      <c r="B4">
-        <v>55</v>
+      <c r="B4" s="1">
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -509,14 +519,15 @@
         <v>2040</v>
       </c>
       <c r="B5">
-        <v>30</v>
+        <f>(B4+B6)/2</f>
+        <v>27.5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2050</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>10</v>
       </c>
     </row>

</xml_diff>